<commit_message>
Archived employees are no longer displayed on the pages, import and export of vacations have been redesigned, and tag filters have been added.
</commit_message>
<xml_diff>
--- a/vacations/export_templates/vacation_template.xlsx
+++ b/vacations/export_templates/vacation_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/konstantin/Проекты/VSCode/Projects/Vacations/vacations/export_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA3C2E2-966F-1B41-8EB7-B8E226BA70A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3692638D-434B-F641-BEB2-641461CF8643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19800" xr2:uid="{009574C5-B610-2E43-83BE-F1203396278F}"/>
   </bookViews>
@@ -111,7 +111,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -120,7 +120,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -458,7 +457,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -542,8 +541,8 @@
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
@@ -556,8 +555,8 @@
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>